<commit_message>
pushed results for first interviewee
</commit_message>
<xml_diff>
--- a/doc/final_presentation/evaluation_results.xlsx
+++ b/doc/final_presentation/evaluation_results.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="TEMPLATE" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="31">
   <si>
     <t>Q1</t>
   </si>
@@ -71,6 +71,53 @@
   </si>
   <si>
     <t>General feedback from the tester (improvements?)</t>
+  </si>
+  <si>
+    <t>Age</t>
+  </si>
+  <si>
+    <t>Sex</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>Candidate</t>
+  </si>
+  <si>
+    <t>M/F</t>
+  </si>
+  <si>
+    <t>&lt;number&gt;</t>
+  </si>
+  <si>
+    <t>Value</t>
+  </si>
+  <si>
+    <t>Masters</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>finding filter was not so obvious obvious one has to look at ban</t>
+  </si>
+  <si>
+    <t>started adding the BAN for different continents but did not immediatly notice the 'total' BAN</t>
+  </si>
+  <si>
+    <t>time slider obvious
+finding country not obvious as you first have to select continent &amp; subregion</t>
+  </si>
+  <si>
+    <t>finding south africa now was easy after having done Q3
+ranked bar chart is obvious</t>
+  </si>
+  <si>
+    <t>No, did not reset the time slider</t>
   </si>
 </sst>
 </file>
@@ -194,7 +241,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -210,6 +257,9 @@
       <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="20" fontId="4" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
   </cellXfs>
@@ -495,10 +545,10 @@
   <sheetPr>
     <tabColor theme="4" tint="-0.249977111117893"/>
   </sheetPr>
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7:F7"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A14" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -510,58 +560,48 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="16.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="1"/>
+      <c r="A1" s="1" t="s">
+        <v>19</v>
+      </c>
       <c r="B1" s="2" t="s">
         <v>13</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="17.399999999999999" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4"/>
-    </row>
-    <row r="3" spans="1:6" ht="33" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" s="5"/>
-      <c r="D3" s="5"/>
-      <c r="E3" s="5"/>
-      <c r="F3" s="5"/>
+      <c r="A2" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2" s="6">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="16.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="4" spans="1:6" ht="16.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="6" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="C4" s="6"/>
-      <c r="D4" s="6"/>
-      <c r="E4" s="6"/>
-      <c r="F4" s="6"/>
+        <v>12</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="5" spans="1:6" ht="33" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="6" t="s">
@@ -571,33 +611,73 @@
         <v>14</v>
       </c>
       <c r="C5" s="6"/>
-      <c r="D5" s="6"/>
-      <c r="E5" s="6"/>
-      <c r="F5" s="6"/>
-    </row>
-    <row r="6" spans="1:6" ht="16.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="B6" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="C6" s="6"/>
-      <c r="D6" s="6"/>
-      <c r="E6" s="6"/>
-      <c r="F6" s="6"/>
-    </row>
-    <row r="7" spans="1:6" ht="33" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="5" t="s">
+    </row>
+    <row r="6" spans="1:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="7" spans="1:6" ht="16.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="1"/>
+      <c r="B7" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="17.399999999999999" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C8" s="4"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="4"/>
+      <c r="F8" s="4"/>
+    </row>
+    <row r="9" spans="1:6" ht="33" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" s="5"/>
+      <c r="D9" s="5"/>
+      <c r="E9" s="5"/>
+      <c r="F9" s="5"/>
+    </row>
+    <row r="10" spans="1:6" ht="16.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C10" s="6"/>
+      <c r="D10" s="6"/>
+      <c r="E10" s="6"/>
+      <c r="F10" s="6"/>
+    </row>
+    <row r="11" spans="1:6" ht="33" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="B11" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="5"/>
-      <c r="D7" s="5"/>
-      <c r="E7" s="5"/>
-      <c r="F7" s="5"/>
+      <c r="C11" s="5"/>
+      <c r="D11" s="5"/>
+      <c r="E11" s="5"/>
+      <c r="F11" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -609,12 +689,175 @@
   <sheetPr>
     <tabColor theme="7" tint="0.39997558519241921"/>
   </sheetPr>
-  <dimension ref="A1"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="53.21875" style="3" customWidth="1"/>
+    <col min="2" max="2" width="35.77734375" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="6" width="27.6640625" style="3" customWidth="1"/>
+    <col min="7" max="16384" width="8.88671875" style="3"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="16.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="17.399999999999999" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2" s="6">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="16.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="16.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="33" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" s="7">
+        <v>0.2986111111111111</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="7" spans="1:6" ht="16.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="1"/>
+      <c r="B7" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="17.399999999999999" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="33" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="F9" s="5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="33" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="E10" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="F10" s="6" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="97.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="F11" s="5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Updated the evaluation results slide
Took 1 interview and updated the feedback
</commit_message>
<xml_diff>
--- a/doc/final_presentation/evaluation_results.xlsx
+++ b/doc/final_presentation/evaluation_results.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10512"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5023DC2A-C075-4040-A681-9F20AD1CE739}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TEMPLATE" sheetId="1" r:id="rId1"/>
@@ -23,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="37">
   <si>
     <t>Q1</t>
   </si>
@@ -118,12 +119,30 @@
   </si>
   <si>
     <t>No, did not reset the time slider</t>
+  </si>
+  <si>
+    <t>yes</t>
+  </si>
+  <si>
+    <t>partly</t>
+  </si>
+  <si>
+    <t>no</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The answer to this question can be given by using the 'status' filter or using the timeslider. Both give slightly different answers. </t>
+  </si>
+  <si>
+    <t>No feedback</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sub region has to be chosen first in order to select a country. Not everyone knows in which sub region a specific country is located. </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -541,7 +560,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <tabColor theme="4" tint="-0.249977111117893"/>
   </sheetPr>
@@ -551,15 +570,15 @@
       <selection activeCell="A14" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="53.21875" style="3" customWidth="1"/>
-    <col min="2" max="2" width="35.77734375" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="53.1640625" style="3" customWidth="1"/>
+    <col min="2" max="2" width="35.83203125" style="3" bestFit="1" customWidth="1"/>
     <col min="3" max="6" width="27.6640625" style="3" customWidth="1"/>
-    <col min="7" max="16384" width="8.88671875" style="3"/>
+    <col min="7" max="16384" width="8.83203125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="16.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>19</v>
       </c>
@@ -570,7 +589,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="17.399999999999999" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" ht="19" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>16</v>
       </c>
@@ -581,7 +600,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="16.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>17</v>
       </c>
@@ -592,7 +611,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="16.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>11</v>
       </c>
@@ -603,7 +622,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="33" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" ht="35" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>10</v>
       </c>
@@ -612,8 +631,8 @@
       </c>
       <c r="C5" s="6"/>
     </row>
-    <row r="6" spans="1:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="7" spans="1:6" ht="16.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="7" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
       <c r="B7" s="2" t="s">
         <v>13</v>
@@ -631,7 +650,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="17.399999999999999" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:6" ht="19" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>3</v>
       </c>
@@ -643,7 +662,7 @@
       <c r="E8" s="4"/>
       <c r="F8" s="4"/>
     </row>
-    <row r="9" spans="1:6" ht="33" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>5</v>
       </c>
@@ -655,7 +674,7 @@
       <c r="E9" s="5"/>
       <c r="F9" s="5"/>
     </row>
-    <row r="10" spans="1:6" ht="16.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
         <v>7</v>
       </c>
@@ -667,7 +686,7 @@
       <c r="E10" s="6"/>
       <c r="F10" s="6"/>
     </row>
-    <row r="11" spans="1:6" ht="33" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
         <v>15</v>
       </c>
@@ -685,25 +704,205 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <sheetPr>
+    <tabColor theme="7" tint="0.39997558519241921"/>
+  </sheetPr>
+  <dimension ref="A1:F11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="53.1640625" style="3" customWidth="1"/>
+    <col min="2" max="2" width="35.83203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="6" width="27.6640625" style="3" customWidth="1"/>
+    <col min="7" max="16384" width="8.83203125" style="3"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="19" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2" s="6">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="35" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" s="7">
+        <v>0.2986111111111111</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="7" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="1"/>
+      <c r="B7" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="19" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="F9" s="5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="35" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="E10" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="F10" s="6" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="69" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="F11" s="5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <tabColor theme="7" tint="0.39997558519241921"/>
   </sheetPr>
   <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="53.21875" style="3" customWidth="1"/>
-    <col min="2" max="2" width="35.77734375" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="6" width="27.6640625" style="3" customWidth="1"/>
-    <col min="7" max="16384" width="8.88671875" style="3"/>
+    <col min="1" max="1" width="28.6640625" customWidth="1"/>
+    <col min="2" max="2" width="35.1640625" customWidth="1"/>
+    <col min="3" max="3" width="36.83203125" customWidth="1"/>
+    <col min="4" max="4" width="28.6640625" customWidth="1"/>
+    <col min="5" max="5" width="21.1640625" customWidth="1"/>
+    <col min="6" max="6" width="26.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="16.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" ht="35" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>19</v>
       </c>
@@ -713,8 +912,11 @@
       <c r="C1" s="2" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" ht="17.399999999999999" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+    </row>
+    <row r="2" spans="1:6" ht="19" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>16</v>
       </c>
@@ -722,10 +924,13 @@
         <v>21</v>
       </c>
       <c r="C2" s="6">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="16.8" thickBot="1" x14ac:dyDescent="0.35">
+        <v>26</v>
+      </c>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+    </row>
+    <row r="3" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>17</v>
       </c>
@@ -735,8 +940,11 @@
       <c r="C3" s="6" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" ht="16.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+    </row>
+    <row r="4" spans="1:6" ht="32" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>11</v>
       </c>
@@ -746,8 +954,11 @@
       <c r="C4" s="6" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" ht="33" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
+    </row>
+    <row r="5" spans="1:6" ht="28" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>10</v>
       </c>
@@ -755,11 +966,21 @@
         <v>14</v>
       </c>
       <c r="C5" s="7">
-        <v>0.2986111111111111</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="7" spans="1:6" ht="16.8" thickBot="1" x14ac:dyDescent="0.35">
+        <v>0.1736111111111111</v>
+      </c>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+    </row>
+    <row r="6" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="3"/>
+      <c r="B6" s="3"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+    </row>
+    <row r="7" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
       <c r="B7" s="2" t="s">
         <v>13</v>
@@ -777,7 +998,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="17.399999999999999" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:6" ht="65" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>3</v>
       </c>
@@ -785,19 +1006,19 @@
         <v>4</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="33" thickBot="1" x14ac:dyDescent="0.35">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="66" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>5</v>
       </c>
@@ -805,19 +1026,19 @@
         <v>6</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>24</v>
+        <v>33</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>24</v>
+        <v>33</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" ht="33" thickBot="1" x14ac:dyDescent="0.35">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="69" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
         <v>7</v>
       </c>
@@ -825,19 +1046,19 @@
         <v>4</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="F10" s="6" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" ht="97.8" thickBot="1" x14ac:dyDescent="0.35">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="143" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
         <v>15</v>
       </c>
@@ -845,16 +1066,16 @@
         <v>8</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>26</v>
+        <v>35</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>27</v>
+        <v>34</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>28</v>
+        <v>36</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -862,8 +1083,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr>
     <tabColor theme="7" tint="0.39997558519241921"/>
   </sheetPr>
@@ -871,29 +1092,14 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
-    <tabColor theme="7" tint="0.39997558519241921"/>
-  </sheetPr>
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <sheetPr>
     <tabColor theme="9" tint="-0.249977111117893"/>
   </sheetPr>
@@ -901,7 +1107,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
added evalution of Person 3
</commit_message>
<xml_diff>
--- a/doc/final_presentation/evaluation_results.xlsx
+++ b/doc/final_presentation/evaluation_results.xlsx
@@ -1,17 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10512"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27531"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5023DC2A-C075-4040-A681-9F20AD1CE739}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADD328FC-E1A1-4C53-9003-9955F5440803}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TEMPLATE" sheetId="1" r:id="rId1"/>
     <sheet name="PERSON 1" sheetId="2" r:id="rId2"/>
     <sheet name="PERSON 2" sheetId="3" r:id="rId3"/>
-    <sheet name="PERSON 3" sheetId="4" r:id="rId4"/>
+    <sheet name="PERSON 3" sheetId="6" r:id="rId4"/>
     <sheet name="SUMMARY" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="162913"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="44">
   <si>
     <t>Q1</t>
   </si>
@@ -137,6 +137,27 @@
   </si>
   <si>
     <t xml:space="preserve">Sub region has to be chosen first in order to select a country. Not everyone knows in which sub region a specific country is located. </t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>Partly</t>
+  </si>
+  <si>
+    <t>Only issue was uncertainty about 'currently': unclear that only 'operating' should be selected.</t>
+  </si>
+  <si>
+    <t>Partly (south of region Africa or country South Africa?; future or current?)</t>
+  </si>
+  <si>
+    <t>Selecting country directly would be helpful.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Unclear to first select a subregion before being able to select country. Would be better to directly be able to select a country.  </t>
+  </si>
+  <si>
+    <t>Clear question and easy to find answer. More info when hovering about time slider would be helpful.</t>
   </si>
 </sst>
 </file>
@@ -283,7 +304,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -567,18 +588,18 @@
   <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A14" sqref="A1:XFD1048576"/>
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="53.1640625" style="3" customWidth="1"/>
-    <col min="2" max="2" width="35.83203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="53.109375" style="3" customWidth="1"/>
+    <col min="2" max="2" width="35.77734375" style="3" bestFit="1" customWidth="1"/>
     <col min="3" max="6" width="27.6640625" style="3" customWidth="1"/>
-    <col min="7" max="16384" width="8.83203125" style="3"/>
+    <col min="7" max="16384" width="8.77734375" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" ht="16.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>19</v>
       </c>
@@ -589,7 +610,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="19" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="17.399999999999999" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="6" t="s">
         <v>16</v>
       </c>
@@ -600,7 +621,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" ht="16.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="6" t="s">
         <v>17</v>
       </c>
@@ -611,7 +632,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" ht="16.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="6" t="s">
         <v>11</v>
       </c>
@@ -622,7 +643,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="35" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" ht="33" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="6" t="s">
         <v>10</v>
       </c>
@@ -631,8 +652,8 @@
       </c>
       <c r="C5" s="6"/>
     </row>
-    <row r="6" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="7" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="7" spans="1:6" ht="16.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="1"/>
       <c r="B7" s="2" t="s">
         <v>13</v>
@@ -650,7 +671,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="19" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" ht="17.399999999999999" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="4" t="s">
         <v>3</v>
       </c>
@@ -662,7 +683,7 @@
       <c r="E8" s="4"/>
       <c r="F8" s="4"/>
     </row>
-    <row r="9" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" ht="33" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="5" t="s">
         <v>5</v>
       </c>
@@ -674,7 +695,7 @@
       <c r="E9" s="5"/>
       <c r="F9" s="5"/>
     </row>
-    <row r="10" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" ht="16.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="6" t="s">
         <v>7</v>
       </c>
@@ -686,7 +707,7 @@
       <c r="E10" s="6"/>
       <c r="F10" s="6"/>
     </row>
-    <row r="11" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" ht="33" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="5" t="s">
         <v>15</v>
       </c>
@@ -711,18 +732,18 @@
   <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="53.1640625" style="3" customWidth="1"/>
-    <col min="2" max="2" width="35.83203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="53.109375" style="3" customWidth="1"/>
+    <col min="2" max="2" width="35.77734375" style="3" bestFit="1" customWidth="1"/>
     <col min="3" max="6" width="27.6640625" style="3" customWidth="1"/>
-    <col min="7" max="16384" width="8.83203125" style="3"/>
+    <col min="7" max="16384" width="8.77734375" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" ht="16.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>19</v>
       </c>
@@ -733,7 +754,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="19" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="17.399999999999999" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="6" t="s">
         <v>16</v>
       </c>
@@ -744,7 +765,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" ht="16.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="6" t="s">
         <v>17</v>
       </c>
@@ -755,7 +776,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" ht="16.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="6" t="s">
         <v>11</v>
       </c>
@@ -766,7 +787,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="35" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" ht="33" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="6" t="s">
         <v>10</v>
       </c>
@@ -777,8 +798,8 @@
         <v>0.2986111111111111</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="7" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="7" spans="1:6" ht="16.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="1"/>
       <c r="B7" s="2" t="s">
         <v>13</v>
@@ -796,7 +817,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="19" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" ht="17.399999999999999" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="4" t="s">
         <v>3</v>
       </c>
@@ -816,7 +837,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" ht="33" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="5" t="s">
         <v>5</v>
       </c>
@@ -836,7 +857,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="35" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" ht="33" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="6" t="s">
         <v>7</v>
       </c>
@@ -856,7 +877,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="69" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" ht="97.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="5" t="s">
         <v>15</v>
       </c>
@@ -888,21 +909,21 @@
   </sheetPr>
   <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="28.6640625" customWidth="1"/>
-    <col min="2" max="2" width="35.1640625" customWidth="1"/>
-    <col min="3" max="3" width="36.83203125" customWidth="1"/>
+    <col min="2" max="2" width="35.109375" customWidth="1"/>
+    <col min="3" max="3" width="36.77734375" customWidth="1"/>
     <col min="4" max="4" width="28.6640625" customWidth="1"/>
-    <col min="5" max="5" width="21.1640625" customWidth="1"/>
-    <col min="6" max="6" width="26.83203125" customWidth="1"/>
+    <col min="5" max="5" width="21.109375" customWidth="1"/>
+    <col min="6" max="6" width="26.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="35" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" ht="16.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>19</v>
       </c>
@@ -916,7 +937,7 @@
       <c r="E1" s="3"/>
       <c r="F1" s="3"/>
     </row>
-    <row r="2" spans="1:6" ht="19" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="17.399999999999999" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="6" t="s">
         <v>16</v>
       </c>
@@ -930,7 +951,7 @@
       <c r="E2" s="3"/>
       <c r="F2" s="3"/>
     </row>
-    <row r="3" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" ht="16.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="6" t="s">
         <v>17</v>
       </c>
@@ -944,7 +965,7 @@
       <c r="E3" s="3"/>
       <c r="F3" s="3"/>
     </row>
-    <row r="4" spans="1:6" ht="32" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" ht="31.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="6" t="s">
         <v>11</v>
       </c>
@@ -958,7 +979,7 @@
       <c r="E4" s="3"/>
       <c r="F4" s="3"/>
     </row>
-    <row r="5" spans="1:6" ht="28" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" ht="28.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="6" t="s">
         <v>10</v>
       </c>
@@ -972,7 +993,7 @@
       <c r="E5" s="3"/>
       <c r="F5" s="3"/>
     </row>
-    <row r="6" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="3"/>
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
@@ -980,7 +1001,7 @@
       <c r="E6" s="3"/>
       <c r="F6" s="3"/>
     </row>
-    <row r="7" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" ht="16.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="1"/>
       <c r="B7" s="2" t="s">
         <v>13</v>
@@ -998,7 +1019,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="65" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" ht="64.95" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="4" t="s">
         <v>3</v>
       </c>
@@ -1018,7 +1039,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="66" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" ht="66" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="5" t="s">
         <v>5</v>
       </c>
@@ -1038,7 +1059,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="69" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" ht="69" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="6" t="s">
         <v>7</v>
       </c>
@@ -1058,7 +1079,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="143" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" ht="142.94999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="5" t="s">
         <v>15</v>
       </c>
@@ -1084,16 +1105,203 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EEBE700E-A60E-484D-A282-8EB5D0D72045}">
   <sheetPr>
     <tabColor theme="7" tint="0.39997558519241921"/>
   </sheetPr>
-  <dimension ref="A1"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <sheetData/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="28.6640625" customWidth="1"/>
+    <col min="2" max="2" width="35.109375" customWidth="1"/>
+    <col min="3" max="3" width="36.77734375" customWidth="1"/>
+    <col min="4" max="4" width="28.6640625" customWidth="1"/>
+    <col min="5" max="5" width="21.109375" customWidth="1"/>
+    <col min="6" max="6" width="26.77734375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="16.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+    </row>
+    <row r="2" spans="1:6" ht="17.399999999999999" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2" s="6">
+        <v>28</v>
+      </c>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+    </row>
+    <row r="3" spans="1:6" ht="16.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+    </row>
+    <row r="4" spans="1:6" ht="31.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
+    </row>
+    <row r="5" spans="1:6" ht="28.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" s="7">
+        <v>0.39374999999999999</v>
+      </c>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+    </row>
+    <row r="6" spans="1:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="3"/>
+      <c r="B6" s="3"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+    </row>
+    <row r="7" spans="1:6" ht="16.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="1"/>
+      <c r="B7" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="64.95" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="66" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="F9" s="5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="69" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="E10" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="F10" s="6" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="142.94999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="F11" s="5" t="s">
+        <v>41</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -1107,7 +1315,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Updated the final presentation slides
Added a diverging stacked bar chart
</commit_message>
<xml_diff>
--- a/doc/final_presentation/evaluation_results.xlsx
+++ b/doc/final_presentation/evaluation_results.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10512"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADD328FC-E1A1-4C53-9003-9955F5440803}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E03A569-C2E6-6C4E-89ED-1A747BD82B3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TEMPLATE" sheetId="1" r:id="rId1"/>
@@ -304,7 +304,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -591,15 +591,15 @@
       <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="53.109375" style="3" customWidth="1"/>
-    <col min="2" max="2" width="35.77734375" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="53.1640625" style="3" customWidth="1"/>
+    <col min="2" max="2" width="35.83203125" style="3" bestFit="1" customWidth="1"/>
     <col min="3" max="6" width="27.6640625" style="3" customWidth="1"/>
-    <col min="7" max="16384" width="8.77734375" style="3"/>
+    <col min="7" max="16384" width="8.83203125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="16.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>19</v>
       </c>
@@ -610,7 +610,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="17.399999999999999" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" ht="19" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>16</v>
       </c>
@@ -621,7 +621,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="16.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>17</v>
       </c>
@@ -632,7 +632,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="16.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>11</v>
       </c>
@@ -643,7 +643,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="33" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" ht="35" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>10</v>
       </c>
@@ -652,8 +652,8 @@
       </c>
       <c r="C5" s="6"/>
     </row>
-    <row r="6" spans="1:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="7" spans="1:6" ht="16.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="7" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
       <c r="B7" s="2" t="s">
         <v>13</v>
@@ -671,7 +671,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="17.399999999999999" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:6" ht="19" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>3</v>
       </c>
@@ -683,7 +683,7 @@
       <c r="E8" s="4"/>
       <c r="F8" s="4"/>
     </row>
-    <row r="9" spans="1:6" ht="33" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>5</v>
       </c>
@@ -695,7 +695,7 @@
       <c r="E9" s="5"/>
       <c r="F9" s="5"/>
     </row>
-    <row r="10" spans="1:6" ht="16.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
         <v>7</v>
       </c>
@@ -707,7 +707,7 @@
       <c r="E10" s="6"/>
       <c r="F10" s="6"/>
     </row>
-    <row r="11" spans="1:6" ht="33" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
         <v>15</v>
       </c>
@@ -732,18 +732,18 @@
   <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="53.109375" style="3" customWidth="1"/>
-    <col min="2" max="2" width="35.77734375" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="53.1640625" style="3" customWidth="1"/>
+    <col min="2" max="2" width="35.83203125" style="3" bestFit="1" customWidth="1"/>
     <col min="3" max="6" width="27.6640625" style="3" customWidth="1"/>
-    <col min="7" max="16384" width="8.77734375" style="3"/>
+    <col min="7" max="16384" width="8.83203125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="16.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>19</v>
       </c>
@@ -754,7 +754,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="17.399999999999999" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" ht="19" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>16</v>
       </c>
@@ -765,7 +765,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="16.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>17</v>
       </c>
@@ -776,7 +776,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="16.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>11</v>
       </c>
@@ -787,7 +787,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="33" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" ht="35" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>10</v>
       </c>
@@ -798,8 +798,8 @@
         <v>0.2986111111111111</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="7" spans="1:6" ht="16.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="7" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
       <c r="B7" s="2" t="s">
         <v>13</v>
@@ -817,7 +817,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="17.399999999999999" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:6" ht="19" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>3</v>
       </c>
@@ -837,7 +837,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="33" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>5</v>
       </c>
@@ -857,7 +857,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="33" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:6" ht="35" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
         <v>7</v>
       </c>
@@ -877,7 +877,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="97.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:6" ht="69" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
         <v>15</v>
       </c>
@@ -909,21 +909,21 @@
   </sheetPr>
   <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="28.6640625" customWidth="1"/>
-    <col min="2" max="2" width="35.109375" customWidth="1"/>
-    <col min="3" max="3" width="36.77734375" customWidth="1"/>
+    <col min="2" max="2" width="35.1640625" customWidth="1"/>
+    <col min="3" max="3" width="36.83203125" customWidth="1"/>
     <col min="4" max="4" width="28.6640625" customWidth="1"/>
-    <col min="5" max="5" width="21.109375" customWidth="1"/>
-    <col min="6" max="6" width="26.77734375" customWidth="1"/>
+    <col min="5" max="5" width="21.1640625" customWidth="1"/>
+    <col min="6" max="6" width="26.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="16.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>19</v>
       </c>
@@ -937,7 +937,7 @@
       <c r="E1" s="3"/>
       <c r="F1" s="3"/>
     </row>
-    <row r="2" spans="1:6" ht="17.399999999999999" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" ht="19" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>16</v>
       </c>
@@ -951,7 +951,7 @@
       <c r="E2" s="3"/>
       <c r="F2" s="3"/>
     </row>
-    <row r="3" spans="1:6" ht="16.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>17</v>
       </c>
@@ -965,7 +965,7 @@
       <c r="E3" s="3"/>
       <c r="F3" s="3"/>
     </row>
-    <row r="4" spans="1:6" ht="31.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" ht="32" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>11</v>
       </c>
@@ -979,7 +979,7 @@
       <c r="E4" s="3"/>
       <c r="F4" s="3"/>
     </row>
-    <row r="5" spans="1:6" ht="28.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" ht="28" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>10</v>
       </c>
@@ -993,7 +993,7 @@
       <c r="E5" s="3"/>
       <c r="F5" s="3"/>
     </row>
-    <row r="6" spans="1:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3"/>
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
@@ -1001,7 +1001,7 @@
       <c r="E6" s="3"/>
       <c r="F6" s="3"/>
     </row>
-    <row r="7" spans="1:6" ht="16.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
       <c r="B7" s="2" t="s">
         <v>13</v>
@@ -1019,7 +1019,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="64.95" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:6" ht="65" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>3</v>
       </c>
@@ -1039,7 +1039,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="66" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:6" ht="66" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>5</v>
       </c>
@@ -1059,7 +1059,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="69" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:6" ht="69" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
         <v>7</v>
       </c>
@@ -1079,7 +1079,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="142.94999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:6" ht="143" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
         <v>15</v>
       </c>
@@ -1111,21 +1111,21 @@
   </sheetPr>
   <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="28.6640625" customWidth="1"/>
-    <col min="2" max="2" width="35.109375" customWidth="1"/>
-    <col min="3" max="3" width="36.77734375" customWidth="1"/>
+    <col min="2" max="2" width="35.1640625" customWidth="1"/>
+    <col min="3" max="3" width="36.83203125" customWidth="1"/>
     <col min="4" max="4" width="28.6640625" customWidth="1"/>
-    <col min="5" max="5" width="21.109375" customWidth="1"/>
-    <col min="6" max="6" width="26.77734375" customWidth="1"/>
+    <col min="5" max="5" width="21.1640625" customWidth="1"/>
+    <col min="6" max="6" width="26.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="16.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>19</v>
       </c>
@@ -1139,7 +1139,7 @@
       <c r="E1" s="3"/>
       <c r="F1" s="3"/>
     </row>
-    <row r="2" spans="1:6" ht="17.399999999999999" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" ht="19" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>16</v>
       </c>
@@ -1153,7 +1153,7 @@
       <c r="E2" s="3"/>
       <c r="F2" s="3"/>
     </row>
-    <row r="3" spans="1:6" ht="16.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>17</v>
       </c>
@@ -1167,7 +1167,7 @@
       <c r="E3" s="3"/>
       <c r="F3" s="3"/>
     </row>
-    <row r="4" spans="1:6" ht="31.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" ht="32" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>11</v>
       </c>
@@ -1181,7 +1181,7 @@
       <c r="E4" s="3"/>
       <c r="F4" s="3"/>
     </row>
-    <row r="5" spans="1:6" ht="28.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" ht="28" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>10</v>
       </c>
@@ -1195,7 +1195,7 @@
       <c r="E5" s="3"/>
       <c r="F5" s="3"/>
     </row>
-    <row r="6" spans="1:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3"/>
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
@@ -1203,7 +1203,7 @@
       <c r="E6" s="3"/>
       <c r="F6" s="3"/>
     </row>
-    <row r="7" spans="1:6" ht="16.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
       <c r="B7" s="2" t="s">
         <v>13</v>
@@ -1221,7 +1221,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="64.95" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:6" ht="65" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>3</v>
       </c>
@@ -1241,7 +1241,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="66" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:6" ht="66" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>5</v>
       </c>
@@ -1261,7 +1261,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="69" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:6" ht="69" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
         <v>7</v>
       </c>
@@ -1281,7 +1281,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="142.94999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:6" ht="143" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
         <v>15</v>
       </c>
@@ -1315,7 +1315,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>